<commit_message>
Implementação da restrição 4
</commit_message>
<xml_diff>
--- a/Inequação restrição janela - avaliação.xlsx
+++ b/Inequação restrição janela - avaliação.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EDMILSON\Documents\UFSC\UFSC - curso de Sistemas de Informação 2019.2\Fase 8\TCC_EDMILSON DOMINGUES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EDMILSON\Documents\UFSC\UFSC - curso de Sistemas de Informação 2019.2\Fase 8\TCC_Edmilson-Domingues\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{743135A4-51B6-4014-8074-0402633F128B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F6BC3E-C2DD-49A1-B6C7-8C621F9FC651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5ADA5AD7-11BF-4CE7-8082-069D38B7CDE9}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5ADA5AD7-11BF-4CE7-8082-069D38B7CDE9}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -397,7 +397,7 @@
   <dimension ref="A11:Z23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,17 +419,17 @@
         <v>2</v>
       </c>
       <c r="K11">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="L11">
         <v>2</v>
       </c>
       <c r="M11">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O11">
         <f>B11*$J$11+C11*$K$11+D11*$L$11+$M$11</f>
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
@@ -447,7 +447,7 @@
       </c>
       <c r="O12">
         <f t="shared" ref="O12:O18" si="0">B12*$J$11+C12*$K$11+D12*$L$11+$M$11</f>
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
@@ -465,7 +465,7 @@
       </c>
       <c r="O13">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
@@ -483,7 +483,7 @@
       </c>
       <c r="O14">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -511,7 +511,7 @@
       <c r="N15"/>
       <c r="O15">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="P15"/>
       <c r="Q15"/>
@@ -550,7 +550,7 @@
       <c r="N16" s="2"/>
       <c r="O16" s="2">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
@@ -568,7 +568,7 @@
       </c>
       <c r="O17">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
@@ -586,7 +586,7 @@
       </c>
       <c r="O18">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">

</xml_diff>